<commit_message>
feature for adding  deptwise free slot added
</commit_message>
<xml_diff>
--- a/InstructorsOnCampus.xlsx
+++ b/InstructorsOnCampus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t xml:space="preserve">Lal Mohan Saha[20500014]</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t xml:space="preserve">Biswajit Guchhait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranendra Narayan Biswas[20500321]</t>
   </si>
 </sst>
 </file>
@@ -416,8 +419,8 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A63" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A86" activeCellId="0" sqref="A86"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A87" activeCellId="0" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -897,6 +900,11 @@
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>